<commit_message>
idk what i did here
</commit_message>
<xml_diff>
--- a/miflyrelation.xlsx
+++ b/miflyrelation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="46">
   <si>
     <t>Airports</t>
   </si>
@@ -161,7 +161,7 @@
     <t>Dept_Port</t>
   </si>
   <si>
-    <t>Timestamp</t>
+    <t>Time_Stamp</t>
   </si>
 </sst>
 </file>
@@ -308,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -330,9 +330,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -382,8 +379,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1805214" y="1735667"/>
-          <a:ext cx="2426608" cy="1143000"/>
+          <a:off x="1813152" y="1714500"/>
+          <a:ext cx="2442483" cy="1143000"/>
           <a:chOff x="1809750" y="1741714"/>
           <a:chExt cx="2435679" cy="1143000"/>
         </a:xfrm>
@@ -498,8 +495,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4218214" y="4402667"/>
-          <a:ext cx="3660322" cy="571500"/>
+          <a:off x="4242027" y="4381500"/>
+          <a:ext cx="3684134" cy="571500"/>
           <a:chOff x="4231821" y="4408714"/>
           <a:chExt cx="3673929" cy="571500"/>
         </a:xfrm>
@@ -614,8 +611,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5445881" y="4688417"/>
-          <a:ext cx="3604381" cy="1428750"/>
+          <a:off x="5477631" y="4667250"/>
+          <a:ext cx="3628194" cy="1428750"/>
           <a:chOff x="5464069" y="4694464"/>
           <a:chExt cx="3617830" cy="1428750"/>
         </a:xfrm>
@@ -730,8 +727,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1805214" y="9178774"/>
-          <a:ext cx="2433411" cy="748393"/>
+          <a:off x="1813152" y="9157607"/>
+          <a:ext cx="2449286" cy="748393"/>
           <a:chOff x="1808389" y="9176657"/>
           <a:chExt cx="2439761" cy="748393"/>
         </a:xfrm>
@@ -846,8 +843,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1806575" y="9546167"/>
-          <a:ext cx="2432050" cy="1714500"/>
+          <a:off x="1814513" y="9525000"/>
+          <a:ext cx="2447925" cy="1714500"/>
           <a:chOff x="1809750" y="9544050"/>
           <a:chExt cx="2438400" cy="1714500"/>
         </a:xfrm>
@@ -962,8 +959,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4222750" y="11832167"/>
-          <a:ext cx="2417233" cy="762000"/>
+          <a:off x="4246563" y="11811000"/>
+          <a:ext cx="2433108" cy="762000"/>
           <a:chOff x="4222750" y="11832167"/>
           <a:chExt cx="2417233" cy="762000"/>
         </a:xfrm>
@@ -1107,8 +1104,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1809750" y="3450167"/>
-          <a:ext cx="2427816" cy="2667000"/>
+          <a:off x="1817688" y="3429000"/>
+          <a:ext cx="2443691" cy="2667000"/>
           <a:chOff x="1809750" y="3450167"/>
           <a:chExt cx="2427816" cy="2667000"/>
         </a:xfrm>
@@ -1500,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,10 +1677,7 @@
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G35" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1843,11 +1837,11 @@
       </c>
     </row>
     <row r="69" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D69" s="9" t="s">
+      <c r="D69" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E69" s="10"/>
-      <c r="F69" s="11"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
everything updated except incident reports gfdi
</commit_message>
<xml_diff>
--- a/miflyrelation.xlsx
+++ b/miflyrelation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="48">
   <si>
     <t>Airports</t>
   </si>
@@ -140,18 +140,12 @@
     <t>0…1</t>
   </si>
   <si>
-    <t>Date_Filed</t>
-  </si>
-  <si>
     <t>Arr_Port</t>
   </si>
   <si>
     <t>Dept_Port</t>
   </si>
   <si>
-    <t>Time_Stamp</t>
-  </si>
-  <si>
     <t>Crew_Num</t>
   </si>
   <si>
@@ -167,7 +161,13 @@
     <t>Reported_FAA</t>
   </si>
   <si>
-    <t>Address</t>
+    <t>Arr_Time</t>
+  </si>
+  <si>
+    <t>Dept_Time</t>
+  </si>
+  <si>
+    <t>Area</t>
   </si>
 </sst>
 </file>
@@ -616,122 +616,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>619881</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>604762</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="36" name="Group 35"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="5477631" y="3357563"/>
-          <a:ext cx="3628194" cy="1238250"/>
-          <a:chOff x="5464069" y="4694464"/>
-          <a:chExt cx="3617830" cy="1428750"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="31" name="Straight Connector 30"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5464069" y="4694464"/>
-            <a:ext cx="0" cy="1047750"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="33" name="Straight Connector 32"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5468622" y="5742214"/>
-            <a:ext cx="3611760" cy="0"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="35" name="Straight Connector 34"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9081899" y="5742214"/>
-            <a:ext cx="0" cy="381000"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>598714</xdr:colOff>
       <xdr:row>38</xdr:row>
@@ -1285,166 +1169,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>607219</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>-1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>607219</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>11906</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Connector 2"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10322719" y="6691312"/>
-          <a:ext cx="0" cy="773907"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>11906</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>642937</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>-1</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="13" name="Group 12"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="7905750" y="6322219"/>
-          <a:ext cx="2452687" cy="2655093"/>
-          <a:chOff x="7905750" y="8036719"/>
-          <a:chExt cx="2452687" cy="3226593"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="7" name="Straight Connector 6"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipV="1">
-            <a:off x="7905750" y="9358312"/>
-            <a:ext cx="0" cy="1905000"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="9" name="Straight Connector 8"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="7905750" y="9358312"/>
-            <a:ext cx="2452687" cy="0"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="12" name="Straight Connector 11"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipV="1">
-            <a:off x="10346531" y="8036719"/>
-            <a:ext cx="0" cy="1321593"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>607219</xdr:colOff>
       <xdr:row>27</xdr:row>
@@ -1557,6 +1281,762 @@
         </xdr:style>
       </xdr:cxnSp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>607218</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="15" name="Group 14"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="10334625" y="5167312"/>
+          <a:ext cx="1202531" cy="1524000"/>
+          <a:chOff x="10334625" y="5167312"/>
+          <a:chExt cx="1202531" cy="1524000"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="4" name="Straight Connector 3"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="10334625" y="5929312"/>
+            <a:ext cx="0" cy="762000"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="6" name="Straight Connector 5"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="11537156" y="5167312"/>
+            <a:ext cx="0" cy="762000"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="10" name="Straight Connector 9"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10334625" y="5929312"/>
+            <a:ext cx="1202531" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>607219</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="27" name="Group 26"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="7893844" y="7262812"/>
+          <a:ext cx="2440781" cy="1714500"/>
+          <a:chOff x="7893844" y="7262812"/>
+          <a:chExt cx="2440781" cy="1714500"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="19" name="Straight Connector 18"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="7893844" y="8024812"/>
+            <a:ext cx="0" cy="952500"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="23" name="Straight Connector 22"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10334625" y="7262812"/>
+            <a:ext cx="0" cy="762000"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="26" name="Straight Connector 25"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7893844" y="8024812"/>
+            <a:ext cx="2440781" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>583406</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="56" name="Group 55"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5441156" y="3357562"/>
+          <a:ext cx="4893469" cy="1238250"/>
+          <a:chOff x="5441156" y="3357562"/>
+          <a:chExt cx="4893469" cy="1238250"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="40" name="Straight Connector 39"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5441156" y="3357562"/>
+            <a:ext cx="0" cy="952500"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="50" name="Straight Connector 49"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5441156" y="4310062"/>
+            <a:ext cx="4893469" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="53" name="Straight Connector 52"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10334625" y="4310062"/>
+            <a:ext cx="0" cy="285750"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>631031</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>619124</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="59" name="Straight Connector 58"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4274344" y="5453062"/>
+          <a:ext cx="2416968" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>619124</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>619124</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="64" name="Straight Connector 63"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6691312" y="5453062"/>
+          <a:ext cx="0" cy="2964657"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>619124</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>619124</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>83343</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="75" name="Straight Connector 74"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9120187" y="8417719"/>
+          <a:ext cx="0" cy="1404937"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>619124</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="77" name="Straight Connector 76"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7905750" y="9834562"/>
+          <a:ext cx="1214437" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="79" name="Straight Connector 78"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7905750" y="9834562"/>
+          <a:ext cx="0" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>619124</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="81" name="Straight Connector 80"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6663836" y="8408560"/>
+          <a:ext cx="1113693" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>690562</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>619124</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="84" name="Straight Connector 83"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7977187" y="8417719"/>
+          <a:ext cx="1143000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>520211</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>163940</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>703384</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>14654</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="90" name="Freeform 89"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7773865" y="8370094"/>
+          <a:ext cx="183173" cy="41214"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 183173"/>
+            <a:gd name="connsiteY0" fmla="*/ 41214 h 41214"/>
+            <a:gd name="connsiteX1" fmla="*/ 58616 w 183173"/>
+            <a:gd name="connsiteY1" fmla="*/ 4579 h 41214"/>
+            <a:gd name="connsiteX2" fmla="*/ 124558 w 183173"/>
+            <a:gd name="connsiteY2" fmla="*/ 4579 h 41214"/>
+            <a:gd name="connsiteX3" fmla="*/ 183173 w 183173"/>
+            <a:gd name="connsiteY3" fmla="*/ 41214 h 41214"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="183173" h="41214">
+              <a:moveTo>
+                <a:pt x="0" y="41214"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="18928" y="25949"/>
+                <a:pt x="37856" y="10685"/>
+                <a:pt x="58616" y="4579"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="79376" y="-1527"/>
+                <a:pt x="103799" y="-1527"/>
+                <a:pt x="124558" y="4579"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="145317" y="10685"/>
+                <a:pt x="164245" y="25949"/>
+                <a:pt x="183173" y="41214"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1830,9 +2310,7 @@
   </sheetPr>
   <dimension ref="B3:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1847,7 +2325,7 @@
     </row>
     <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1881,10 +2359,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -1968,7 +2446,8 @@
       <c r="D24" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="E24" s="7"/>
+      <c r="I24" s="7" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1982,7 +2461,8 @@
       <c r="D25" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="E25" s="7"/>
+      <c r="I25" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1991,32 +2471,35 @@
         <v>6</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="J27" s="8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2024,7 +2507,7 @@
       <c r="B28" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I28" s="7" t="s">
+      <c r="J28" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2032,51 +2515,33 @@
       <c r="D30" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I30" s="7" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C31" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H31" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C32" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C33" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I33" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I34" s="7" t="s">
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="7" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2084,6 +2549,12 @@
       <c r="B36" s="10" t="s">
         <v>22</v>
       </c>
+      <c r="H36" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
@@ -2095,16 +2566,28 @@
       <c r="D37" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="H37" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="I38" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="I39" s="7" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D41" s="7" t="s">
@@ -2168,7 +2651,7 @@
         <v>30</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
@@ -2189,6 +2672,9 @@
       <c r="F53" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="G53" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D54" s="10" t="s">
@@ -2200,34 +2686,37 @@
       <c r="F54" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="G54" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D55" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H55" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H55" s="2" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D56" s="11" t="s">
+      <c r="E56" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E56" s="12"/>
-      <c r="F56" s="13"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="E56:G56"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="64" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>